<commit_message>
Exclude test pads, graphics, etc., from BOM
</commit_message>
<xml_diff>
--- a/r1/build/tr23-r1-bom/tr23-badge-r1.xlsx
+++ b/r1/build/tr23-r1-bom/tr23-badge-r1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="254">
   <si>
     <t xml:space="preserve">Ref</t>
   </si>
@@ -77,16 +77,7 @@
     <t xml:space="preserve">C503591</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:ESP32-WROVER-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AE1, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antenna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jeffmakes_footprints:Antenna_TI_DN038</t>
+    <t xml:space="preserve">jeffmakes-footprints:ESP32-WROVER-I</t>
   </si>
   <si>
     <t xml:space="preserve">C1, C2, </t>
@@ -104,7 +95,7 @@
     <t xml:space="preserve">Unpolarized capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C3, C5, C11, C12, C14, C18, C19, C31, C32, C33, C34, C35, C36, C38, C39, C40, </t>
+    <t xml:space="preserve">C3, C5, C11, C12, C14, C18, C19, C31, C32, C33, C34, C35, C36, C38, C39, C40, C70, C71, C72, </t>
   </si>
   <si>
     <t xml:space="preserve">100nF</t>
@@ -221,7 +212,7 @@
     <t xml:space="preserve">C99881</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:D-1206</t>
+    <t xml:space="preserve">jeffmakes-footprints:D-1206</t>
   </si>
   <si>
     <t xml:space="preserve">Light emitting diode</t>
@@ -278,25 +269,13 @@
     <t xml:space="preserve">C261278</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:SOD-523-numbered-pads</t>
+    <t xml:space="preserve">jeffmakes-footprints:SOD-523-numbered-pads</t>
   </si>
   <si>
     <t xml:space="preserve">Bidirectional transient-voltage-suppression diode</t>
   </si>
   <si>
-    <t xml:space="preserve">FID1, FID2, FID3, FID4, FID5, FID6, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiducial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiducial:Fiducial_1mm_Mask2mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fiducial Marker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1, </t>
+    <t xml:space="preserve">J1, J9, </t>
   </si>
   <si>
     <t xml:space="preserve">Molex</t>
@@ -326,7 +305,7 @@
     <t xml:space="preserve">C283540</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:jing-usb-c-lcsc-C167321</t>
+    <t xml:space="preserve">jeffmakes-footprints:jing-usb-c-lcsc-C167321</t>
   </si>
   <si>
     <t xml:space="preserve">J3, </t>
@@ -335,7 +314,7 @@
     <t xml:space="preserve">USB-A-10mm-flangeless</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:USB-A-short-body</t>
+    <t xml:space="preserve">jeffmakes-footprints:USB-A-short-body</t>
   </si>
   <si>
     <t xml:space="preserve">USB Type A connector</t>
@@ -356,7 +335,7 @@
     <t xml:space="preserve">C262648</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:AFC07x40-1MP_P0.5mm_Horizontal</t>
+    <t xml:space="preserve">jeffmakes-footprints:AFC07x40-1MP_P0.5mm_Horizontal_reverse_pinout</t>
   </si>
   <si>
     <t xml:space="preserve">Generic connectable mounting pin connector, single row, 01x40, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -371,7 +350,7 @@
     <t xml:space="preserve">C431535</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:Jack_3.5mm_PJ320D_Horizontal_strengthening-vias</t>
+    <t xml:space="preserve">jeffmakes-footprints:Jack_3.5mm_PJ320D_Horizontal_strengthening-vias</t>
   </si>
   <si>
     <t xml:space="preserve">Audio Jack, 4 Poles (TRRS)</t>
@@ -383,7 +362,7 @@
     <t xml:space="preserve">2x03-socket-2.54-through-board</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:PinSocket_2x03_P2.54mm_Through-Board-Mating</t>
+    <t xml:space="preserve">jeffmakes-footprints:PinSocket_2x03_P2.54mm_Through-Board-Mating</t>
   </si>
   <si>
     <t xml:space="preserve">Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -404,13 +383,13 @@
     <t xml:space="preserve">C111196</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:microSD_HC_Sofng_TF-15</t>
+    <t xml:space="preserve">jeffmakes-footprints:microSD_HC_Sofng_TF-15</t>
   </si>
   <si>
     <t xml:space="preserve">J8, </t>
   </si>
   <si>
-    <t xml:space="preserve">Connector_Coaxial:SMA_Amphenol_132291-12_Vertical</t>
+    <t xml:space="preserve">Connector_Coaxial:SMA_Amphenol_132134-10_Vertical</t>
   </si>
   <si>
     <t xml:space="preserve">coaxial connector (BNC, SMA, SMB, SMC, Cinch/RCA, LEMO, ...)</t>
@@ -485,13 +464,13 @@
     <t xml:space="preserve">C82917</t>
   </si>
   <si>
-    <t xml:space="preserve">LED1, LED2, LED3, LED4, LED5, LED6, </t>
+    <t xml:space="preserve">LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, </t>
   </si>
   <si>
     <t xml:space="preserve">Reverse mount?</t>
   </si>
   <si>
-    <t xml:space="preserve">LED_SMD:LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+    <t xml:space="preserve">jeffmakes-footprints:LED_SK6812SIDE-A</t>
   </si>
   <si>
     <t xml:space="preserve">RGB LED with integrated controller</t>
@@ -572,7 +551,7 @@
     <t xml:space="preserve">56k</t>
   </si>
   <si>
-    <t xml:space="preserve">R29, </t>
+    <t xml:space="preserve">R29, R32, R33, </t>
   </si>
   <si>
     <t xml:space="preserve">10R</t>
@@ -596,7 +575,7 @@
     <t xml:space="preserve">C&amp;K</t>
   </si>
   <si>
-    <t xml:space="preserve">Button_Switch_SMD:SW_SPST_PTS645</t>
+    <t xml:space="preserve">jeffmakes-footprints:SW_SPST_TACT-6x6-no-silk</t>
   </si>
   <si>
     <t xml:space="preserve">Push button switch, generic, two pins</t>
@@ -605,7 +584,7 @@
     <t xml:space="preserve">See Sheet 4 – coloured switches, but must be SMT type</t>
   </si>
   <si>
-    <t xml:space="preserve">S3, </t>
+    <t xml:space="preserve">S3, S8, </t>
   </si>
   <si>
     <t xml:space="preserve">K3-1296S-J1</t>
@@ -614,7 +593,7 @@
     <t xml:space="preserve">C223848</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:SW_JS102011SAQN</t>
+    <t xml:space="preserve">Button_Switch_SMD:SW_SPDT_PCM12</t>
   </si>
   <si>
     <t xml:space="preserve">S5, </t>
@@ -626,40 +605,22 @@
     <t xml:space="preserve">C145899</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:SW_JS1400BFQ-arrows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1, SW2, SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11, SW12, SW13, SW14, SW15, SW16, SW17, SW18, SW19, SW20, SW21, SW22, SW23, SW24, SW25, SW26, SW27, SW28, SW29, SW30, SW31, SW32,  SW33,  SW34, </t>
+    <t xml:space="preserve">jeffmakes-footprints:SW_JS1400BFQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1, SW2, SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11, SW12, SW13, SW14, SW15, SW16, SW17, SW18, SW19, SW20, SW21, SW22, SW23, SW24, SW25, SW26, SW27, SW28, SW29, SW30, SW31, SW32, SW33, SW34, </t>
   </si>
   <si>
     <t xml:space="preserve">REV_TACT</t>
   </si>
   <si>
-    <t xml:space="preserve">jeffmakes_footprints:SW_SPST_TACT_6x6_REV_MOUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEC 5G single pole normally-open tactile switch</t>
+    <t xml:space="preserve">jeffmakes-footprints:SW_SPST_TACT_6x6_REV_MOUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEC 5E single pole normally-open tactile switch</t>
   </si>
   <si>
     <t xml:space="preserve">See Sheet 5 – reverse mount switches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13, TP14, TP15, TP16, TP17, TP18, TP19, TP20, TP21, TP22, TP23, TP24, TP25, TP26, TP27, TP28, TP29, TP30, TP31, TP32, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jeffmakes_footprints:test-pad-1.4-TH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP33, TP34, TP35, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Pad_D1.0mm</t>
   </si>
   <si>
     <t xml:space="preserve">U1, </t>
@@ -839,6 +800,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -860,6 +822,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -910,16 +873,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,9 +925,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>17640</xdr:colOff>
+      <xdr:colOff>17280</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -962,7 +941,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6519960" cy="4673880"/>
+          <a:ext cx="6519600" cy="4673520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -983,9 +962,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>594720</xdr:colOff>
+      <xdr:colOff>594360</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -999,7 +978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6467760" y="0"/>
-          <a:ext cx="6319080" cy="4635360"/>
+          <a:ext cx="6318720" cy="4635000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1020,9 +999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>733680</xdr:colOff>
+      <xdr:colOff>733320</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1036,7 +1015,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4554000"/>
-          <a:ext cx="6423120" cy="4095360"/>
+          <a:ext cx="6422760" cy="4095000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1057,9 +1036,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>601920</xdr:colOff>
+      <xdr:colOff>601560</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1073,7 +1052,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6344280" y="4592520"/>
-          <a:ext cx="6449760" cy="4083840"/>
+          <a:ext cx="6449400" cy="4083480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,9 +1078,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>98640</xdr:colOff>
+      <xdr:colOff>98280</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1115,7 +1094,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="15541920" cy="10413000"/>
+          <a:ext cx="15541560" cy="10412640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1141,9 +1120,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>86040</xdr:colOff>
+      <xdr:colOff>85680</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1157,7 +1136,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="18780480" cy="8088480"/>
+          <a:ext cx="18780120" cy="8088120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,9 +1162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>500040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1199,7 +1178,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6189840" cy="4645440"/>
+          <a:ext cx="6189480" cy="4645080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1220,9 +1199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>484560</xdr:colOff>
+      <xdr:colOff>484200</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1236,7 +1215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5421600" y="0"/>
-          <a:ext cx="11319120" cy="15328080"/>
+          <a:ext cx="11318760" cy="15327720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1257,9 +1236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>554040</xdr:colOff>
+      <xdr:colOff>553680</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1273,7 +1252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16275240" y="0"/>
-          <a:ext cx="15977880" cy="11015640"/>
+          <a:ext cx="15977520" cy="11015280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1293,67 +1272,67 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M71"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D79" activeCellId="0" sqref="D79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="67.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="76.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="171.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="67.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="76.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="171.84"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1367,6 +1346,9 @@
       <c r="C2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
       <c r="G2" s="0" t="s">
         <v>15</v>
       </c>
@@ -1379,645 +1361,866 @@
       <c r="J2" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
       <c r="J3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>25</v>
-      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
       <c r="J6" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>32</v>
-      </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
       <c r="J7" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
       <c r="J8" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
       <c r="J9" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
       <c r="J10" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>41</v>
-      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
       <c r="J11" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>43</v>
-      </c>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
       <c r="J12" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+    </row>
+    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="B14" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
       <c r="J14" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+    </row>
+    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
       <c r="F15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+    </row>
+    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="0"/>
+      <c r="M16" s="0"/>
+    </row>
+    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="0"/>
+      <c r="M17" s="0"/>
+    </row>
+    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+    </row>
+    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="I20" s="0" t="s">
+        <v>61</v>
+      </c>
       <c r="J20" s="0" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
+    </row>
+    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="K21" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+    </row>
+    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="0" t="s">
         <v>69</v>
       </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
       <c r="I22" s="0" t="s">
         <v>70</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+    </row>
+    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>77</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
       <c r="H24" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
+    </row>
+    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>82</v>
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>532610271</v>
+      </c>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>532610271</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+    </row>
+    <row r="26" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+    </row>
+    <row r="27" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+    </row>
+    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>532610271</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>532610271</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="H29" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="J29" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H30" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="I30" s="0" t="s">
+      <c r="K29" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+    </row>
+    <row r="30" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="B30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>113</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
       <c r="G31" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+    </row>
+    <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K32" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+    </row>
+    <row r="33" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>123</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
       <c r="G33" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I33" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+    </row>
+    <row r="34" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="J33" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>36</v>
+      <c r="H34" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>133</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>128</v>
@@ -2025,731 +2228,803 @@
       <c r="K34" s="0" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+    </row>
+    <row r="35" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>131</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
       <c r="G35" s="0" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+    </row>
+    <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>138</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
       <c r="G36" s="0" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="L36" s="0"/>
+      <c r="M36" s="0"/>
+    </row>
+    <row r="37" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>142</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
       <c r="G37" s="0" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="L37" s="0"/>
+      <c r="M37" s="0"/>
+    </row>
+    <row r="38" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="G38" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J38" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="K38" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
+    </row>
+    <row r="39" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>150</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
       <c r="G39" s="0" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="H39" s="0" t="s">
         <v>151</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>155</v>
+      </c>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+    </row>
+    <row r="40" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C40" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="J40" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="J40" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="K40" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>160</v>
+      </c>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
+    </row>
+    <row r="41" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0"/>
+    </row>
+    <row r="42" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+      <c r="J42" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0"/>
+    </row>
+    <row r="43" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+      <c r="J43" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
+    </row>
+    <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+      <c r="J44" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
+    </row>
+    <row r="45" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+      <c r="J45" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+    </row>
+    <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C46" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+    </row>
+    <row r="47" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="J47" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K47" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+    </row>
+    <row r="48" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
+      <c r="G48" s="0"/>
+      <c r="H48" s="0"/>
+      <c r="I48" s="0"/>
+      <c r="J48" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
+    </row>
+    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
+    </row>
+    <row r="51" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
+      <c r="G51" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="K51" s="0"/>
+      <c r="L51" s="0"/>
+      <c r="M51" s="0"/>
+    </row>
+    <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B52" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
+      <c r="F53" s="0"/>
+      <c r="G53" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="L53" s="0"/>
+      <c r="M53" s="0"/>
+    </row>
+    <row r="54" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="0"/>
+      <c r="E54" s="0"/>
+      <c r="F54" s="0"/>
+      <c r="G54" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="G41" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H41" s="0" t="s">
+      <c r="H54" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="I54" s="0"/>
+      <c r="J54" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="K54" s="0"/>
+      <c r="L54" s="0"/>
+      <c r="M54" s="0"/>
+    </row>
+    <row r="55" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="0"/>
+      <c r="E55" s="0"/>
+      <c r="F55" s="0"/>
+      <c r="G55" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="L55" s="0"/>
+      <c r="M55" s="0"/>
+    </row>
+    <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
+      <c r="F56" s="0"/>
+      <c r="G56" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="L56" s="0"/>
+      <c r="M56" s="0"/>
+    </row>
+    <row r="57" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="G57" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="I41" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="K42" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="I43" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="J43" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="K43" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="J44" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="J45" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="J46" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="J47" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K47" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="J48" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K48" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="J49" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K49" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="J50" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="K50" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="51" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B54" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="J55" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="K55" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B56" s="0" t="n">
+      <c r="H57" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+    </row>
+    <row r="58" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B58" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="K56" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="I57" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="J57" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="K57" s="0" t="s">
+      <c r="C58" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="G58" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="H58" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>229</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+      <c r="M58" s="0"/>
+    </row>
+    <row r="59" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>224</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="D59" s="0"/>
+      <c r="E59" s="0"/>
+      <c r="F59" s="0"/>
       <c r="G59" s="0" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>235</v>
+      </c>
+      <c r="L59" s="0"/>
+      <c r="M59" s="0"/>
+    </row>
+    <row r="60" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>230</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="D60" s="0"/>
+      <c r="E60" s="0"/>
+      <c r="F60" s="0"/>
       <c r="G60" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>242</v>
+      </c>
+      <c r="L60" s="0"/>
+      <c r="M60" s="0"/>
+    </row>
+    <row r="61" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>237</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="D61" s="0"/>
+      <c r="E61" s="0"/>
+      <c r="F61" s="0"/>
       <c r="G61" s="0" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="J63" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="K63" s="0" t="s">
+      <c r="K61" s="0" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="L61" s="0"/>
+      <c r="M61" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="0" t="s">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G64" s="0" t="s">
+      <c r="B68" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="H64" s="0" t="s">
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="I64" s="0" t="s">
+      <c r="B69" s="6" t="n">
+        <v>350</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="J64" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="K64" s="0" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="G65" s="0" t="s">
+      <c r="B70" s="6" t="n">
+        <v>350</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="H65" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="I65" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="K65" s="0" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B69" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B70" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B71" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2770,7 +3045,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R29" activeCellId="0" sqref="R29"/>
     </sheetView>
   </sheetViews>
@@ -2794,7 +3069,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V47" activeCellId="0" sqref="V47"/>
     </sheetView>
   </sheetViews>
@@ -2818,7 +3093,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2842,7 +3117,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update BoM to include reverse-mount switch data
</commit_message>
<xml_diff>
--- a/r1/build/tr23-r1-bom/tr23-badge-r1.xlsx
+++ b/r1/build/tr23-r1-bom/tr23-badge-r1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="256">
   <si>
     <t xml:space="preserve">Ref</t>
   </si>
@@ -611,13 +611,19 @@
     <t xml:space="preserve">SW1, SW2, SW3, SW4, SW5, SW6, SW7, SW8, SW9, SW10, SW11, SW12, SW13, SW14, SW15, SW16, SW17, SW18, SW19, SW20, SW21, SW22, SW23, SW24, SW25, SW26, SW27, SW28, SW29, SW30, SW31, SW32, SW33, SW34, </t>
   </si>
   <si>
-    <t xml:space="preserve">REV_TACT</t>
+    <t xml:space="preserve">8HG-P-A-S1-03-065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laxxscom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8HG</t>
   </si>
   <si>
     <t xml:space="preserve">jeffmakes-footprints:SW_SPST_TACT_6x6_REV_MOUNT</t>
   </si>
   <si>
-    <t xml:space="preserve">MEC 5E single pole normally-open tactile switch</t>
+    <t xml:space="preserve">Reverse-mount single pole normally-open tactile switch</t>
   </si>
   <si>
     <t xml:space="preserve">See Sheet 5 – reverse mount switches</t>
@@ -873,12 +879,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1274,8 +1284,8 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1295,44 +1305,44 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="171.84"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1650,7 +1660,7 @@
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
     </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>45</v>
       </c>
@@ -1677,7 +1687,7 @@
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
     </row>
-    <row r="15" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>48</v>
       </c>
@@ -1704,7 +1714,7 @@
       <c r="L15" s="0"/>
       <c r="M15" s="0"/>
     </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>50</v>
       </c>
@@ -1731,7 +1741,7 @@
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
     </row>
-    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>52</v>
       </c>
@@ -1758,7 +1768,7 @@
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
     </row>
-    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>54</v>
       </c>
@@ -1785,7 +1795,7 @@
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
     </row>
-    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>56</v>
       </c>
@@ -1810,7 +1820,7 @@
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>58</v>
       </c>
@@ -1839,7 +1849,7 @@
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
     </row>
-    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>64</v>
       </c>
@@ -1868,7 +1878,7 @@
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
     </row>
-    <row r="22" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>68</v>
       </c>
@@ -1895,7 +1905,7 @@
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
     </row>
-    <row r="23" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>73</v>
       </c>
@@ -1924,7 +1934,7 @@
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
     </row>
-    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>77</v>
       </c>
@@ -1953,7 +1963,7 @@
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
     </row>
-    <row r="25" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>83</v>
       </c>
@@ -1984,7 +1994,7 @@
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
     </row>
-    <row r="26" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>88</v>
       </c>
@@ -2013,27 +2023,27 @@
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
     </row>
-    <row r="27" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+    <row r="27" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>99</v>
       </c>
@@ -2064,7 +2074,7 @@
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
     </row>
-    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>105</v>
       </c>
@@ -2095,27 +2105,27 @@
       <c r="L29" s="0"/>
       <c r="M29" s="0"/>
     </row>
-    <row r="30" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+    <row r="30" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>115</v>
       </c>
@@ -2144,7 +2154,7 @@
       <c r="L31" s="0"/>
       <c r="M31" s="0"/>
     </row>
-    <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>120</v>
       </c>
@@ -2169,7 +2179,7 @@
       <c r="L32" s="0"/>
       <c r="M32" s="0"/>
     </row>
-    <row r="33" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>123</v>
       </c>
@@ -2200,7 +2210,7 @@
       <c r="L33" s="0"/>
       <c r="M33" s="0"/>
     </row>
-    <row r="34" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>130</v>
       </c>
@@ -2231,7 +2241,7 @@
       <c r="L34" s="0"/>
       <c r="M34" s="0"/>
     </row>
-    <row r="35" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>134</v>
       </c>
@@ -2262,7 +2272,7 @@
       <c r="L35" s="0"/>
       <c r="M35" s="0"/>
     </row>
-    <row r="36" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>138</v>
       </c>
@@ -2293,7 +2303,7 @@
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
     </row>
-    <row r="37" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>142</v>
       </c>
@@ -2324,7 +2334,7 @@
       <c r="L37" s="0"/>
       <c r="M37" s="0"/>
     </row>
-    <row r="38" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>146</v>
       </c>
@@ -2349,7 +2359,7 @@
       <c r="L38" s="0"/>
       <c r="M38" s="0"/>
     </row>
-    <row r="39" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>150</v>
       </c>
@@ -2380,7 +2390,7 @@
       <c r="L39" s="0"/>
       <c r="M39" s="0"/>
     </row>
-    <row r="40" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>156</v>
       </c>
@@ -2411,7 +2421,7 @@
       <c r="L40" s="0"/>
       <c r="M40" s="0"/>
     </row>
-    <row r="41" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>161</v>
       </c>
@@ -2440,7 +2450,7 @@
       <c r="L41" s="0"/>
       <c r="M41" s="0"/>
     </row>
-    <row r="42" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>165</v>
       </c>
@@ -2465,7 +2475,7 @@
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
     </row>
-    <row r="43" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>169</v>
       </c>
@@ -2490,7 +2500,7 @@
       <c r="L43" s="0"/>
       <c r="M43" s="0"/>
     </row>
-    <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>171</v>
       </c>
@@ -2515,7 +2525,7 @@
       <c r="L44" s="0"/>
       <c r="M44" s="0"/>
     </row>
-    <row r="45" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>173</v>
       </c>
@@ -2540,7 +2550,7 @@
       <c r="L45" s="0"/>
       <c r="M45" s="0"/>
     </row>
-    <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>175</v>
       </c>
@@ -2565,7 +2575,7 @@
       <c r="L46" s="0"/>
       <c r="M46" s="0"/>
     </row>
-    <row r="47" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>177</v>
       </c>
@@ -2590,7 +2600,7 @@
       <c r="L47" s="0"/>
       <c r="M47" s="0"/>
     </row>
-    <row r="48" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>178</v>
       </c>
@@ -2615,30 +2625,30 @@
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
     </row>
-    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+    <row r="49" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="4" t="n">
+      <c r="B49" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J49" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="K49" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="M49" s="4" t="s">
+      <c r="M49" s="5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="50" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>186</v>
       </c>
@@ -2667,7 +2677,7 @@
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
     </row>
-    <row r="51" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>190</v>
       </c>
@@ -2696,66 +2706,72 @@
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
     </row>
-    <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+    <row r="52" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B52" s="4" t="n">
+      <c r="B52" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="G52" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="K52" s="4" t="s">
+      <c r="H52" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="J52" s="5" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="53" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K52" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
       <c r="G53" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
     </row>
-    <row r="54" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D54" s="0"/>
       <c r="E54" s="0"/>
@@ -2764,87 +2780,87 @@
         <v>158</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="I54" s="0"/>
       <c r="J54" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K54" s="0"/>
       <c r="L54" s="0"/>
       <c r="M54" s="0"/>
     </row>
-    <row r="55" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
       <c r="G55" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
     </row>
-    <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D56" s="0"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
       <c r="G56" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="L56" s="0"/>
       <c r="M56" s="0"/>
     </row>
-    <row r="57" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D57" s="0"/>
       <c r="E57" s="0"/>
@@ -2853,178 +2869,178 @@
         <v>158</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K57" s="0"/>
       <c r="L57" s="0"/>
       <c r="M57" s="0"/>
     </row>
-    <row r="58" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
       <c r="G58" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="K58" s="0"/>
       <c r="L58" s="0"/>
       <c r="M58" s="0"/>
     </row>
-    <row r="59" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D59" s="0"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
       <c r="G59" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
     </row>
-    <row r="60" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D60" s="0"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
       <c r="G60" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
     </row>
-    <row r="61" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
       <c r="G61" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
+      <c r="A67" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B68" s="6" t="n">
+      <c r="A68" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B68" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>251</v>
+      <c r="C68" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B69" s="6" t="n">
+      <c r="A69" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="7" t="n">
         <v>350</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>251</v>
+      <c r="C69" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B70" s="7" t="n">
+        <v>350</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="B70" s="6" t="n">
-        <v>350</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>